<commit_message>
Almost finished. Fixing references and then that it it
Signed-off-by: Callum <callum.terris@gmail.com>
</commit_message>
<xml_diff>
--- a/Documents/results level 2.xlsx
+++ b/Documents/results level 2.xlsx
@@ -240,44 +240,337 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Maximum</c:v>
+          </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:f>Sheet1!$H$1:$H$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$1:$I$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.35</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                <c:pt idx="44">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.45</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,11 +587,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142680064"/>
-        <c:axId val="142681600"/>
+        <c:axId val="38853632"/>
+        <c:axId val="38912768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142680064"/>
+        <c:axId val="38853632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -307,7 +600,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142681600"/>
+        <c:crossAx val="38912768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -315,7 +608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142681600"/>
+        <c:axId val="38912768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,7 +619,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142680064"/>
+        <c:crossAx val="38853632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -348,155 +641,24 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>(Sheet1!$A$2,Sheet1!$A$13,Sheet1!$A$24,Sheet1!$A$35,Sheet1!$A$46,Sheet1!$A$57,Sheet1!$A$68,Sheet1!$A$79,Sheet1!$A$90,Sheet1!$A$101)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="142718080"/>
-        <c:axId val="142719616"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="142718080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142719616"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="142719616"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142718080"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="7" name="Chart 6"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -506,36 +668,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -831,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +975,7 @@
     <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -853,8 +985,14 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1">
+        <v>4</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -864,8 +1002,14 @@
       <c r="F2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -875,8 +1019,14 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -886,8 +1036,14 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -897,8 +1053,14 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -908,8 +1070,14 @@
       <c r="F6">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -919,8 +1087,14 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -930,8 +1104,14 @@
       <c r="F8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -941,8 +1121,14 @@
       <c r="F9">
         <v>1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -952,8 +1138,14 @@
       <c r="F10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -963,8 +1155,14 @@
       <c r="F11">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -974,8 +1172,14 @@
       <c r="F12">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -985,8 +1189,14 @@
       <c r="F13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -996,8 +1206,14 @@
       <c r="F14">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1007,8 +1223,14 @@
       <c r="F15">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1018,8 +1240,14 @@
       <c r="F16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1029,8 +1257,14 @@
       <c r="F17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1040,8 +1274,14 @@
       <c r="F18">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>4</v>
+      </c>
+      <c r="I18">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1051,8 +1291,14 @@
       <c r="F19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1062,8 +1308,14 @@
       <c r="F20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -1073,8 +1325,14 @@
       <c r="F21">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -1084,8 +1342,14 @@
       <c r="F22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1095,8 +1359,14 @@
       <c r="F23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1106,8 +1376,14 @@
       <c r="F24">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1117,8 +1393,14 @@
       <c r="F25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1128,8 +1410,14 @@
       <c r="F26">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1139,8 +1427,14 @@
       <c r="F27">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1150,8 +1444,14 @@
       <c r="F28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1161,8 +1461,14 @@
       <c r="F29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1172,8 +1478,14 @@
       <c r="F30">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1183,8 +1495,14 @@
       <c r="F31" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0</v>
       </c>
@@ -1194,8 +1512,14 @@
       <c r="F32">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1205,8 +1529,14 @@
       <c r="F33">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1216,8 +1546,14 @@
       <c r="F34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1227,8 +1563,14 @@
       <c r="F35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -1238,8 +1580,14 @@
       <c r="F36">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1249,8 +1597,14 @@
       <c r="F37" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1260,8 +1614,14 @@
       <c r="F38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1271,8 +1631,14 @@
       <c r="F39">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>4</v>
+      </c>
+      <c r="I39">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1282,8 +1648,14 @@
       <c r="F40" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>4</v>
+      </c>
+      <c r="I40">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
@@ -1293,8 +1665,14 @@
       <c r="F41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0</v>
       </c>
@@ -1304,8 +1682,14 @@
       <c r="F42">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0</v>
       </c>
@@ -1315,8 +1699,14 @@
       <c r="F43" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0</v>
       </c>
@@ -1326,8 +1716,14 @@
       <c r="F44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1337,8 +1733,14 @@
       <c r="F45">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -1348,8 +1750,14 @@
       <c r="F46" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -1359,8 +1767,14 @@
       <c r="F47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1370,8 +1784,14 @@
       <c r="F48">
         <v>1.45</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1381,8 +1801,14 @@
       <c r="F49" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1392,8 +1818,14 @@
       <c r="F50">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
@@ -1404,7 +1836,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0</v>
       </c>
@@ -1415,7 +1847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0</v>
       </c>
@@ -1426,7 +1858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0</v>
       </c>
@@ -1437,7 +1869,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0</v>
       </c>
@@ -1448,7 +1880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -1459,7 +1891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
@@ -1470,7 +1902,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -1481,7 +1913,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -1492,7 +1924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>3</v>
       </c>
@@ -1503,7 +1935,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1514,7 +1946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1525,7 +1957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1536,7 +1968,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>

</xml_diff>